<commit_message>
Updated trendline equation in Excel
</commit_message>
<xml_diff>
--- a/output/Bruteforce time data.xlsx
+++ b/output/Bruteforce time data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\GitHub\COMP90043_RSA_Attacks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E307DF39-E61A-432C-8053-FB0AD79944AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC56E86-256F-4D4E-8A41-3263CFA2A2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2948" yWindow="1350" windowWidth="23324" windowHeight="13710" xr2:uid="{009308DD-D7FB-4A66-90C8-9029A2463257}"/>
+    <workbookView xWindow="1275" yWindow="1808" windowWidth="23325" windowHeight="13710" xr2:uid="{009308DD-D7FB-4A66-90C8-9029A2463257}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -837,7 +837,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:numFmt formatCode="#,##0.00000" sourceLinked="0"/>
+              <c:numFmt formatCode="#,##0.0000000000" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -2815,8 +2815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41025246-FDA7-4F73-B0A2-EE1A44AFCEA8}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>